<commit_message>
2023-09-21 : Synchronize codes to the origin repository.
</commit_message>
<xml_diff>
--- a/TestData/Book1.xlsx
+++ b/TestData/Book1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Aspose\Aspose for Cloud\Aspose.Cells for Cloud\testdata\Cells\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\test\data\asposecellscloudsdk\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363DEB7A-E329-4687-BF50-318DFD33AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19020" windowHeight="11640" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +19,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="insert" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet8" sheetId="9" r:id="rId7"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId8"/>
+    <sheet name="insert" sheetId="8" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$B$3:$E$18</definedName>
@@ -27,17 +29,30 @@
     <definedName name="Name_3">Sheet2!$D$21:$H$23</definedName>
     <definedName name="TestName1">Sheet1!$O$25:$P$30</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roy Wang</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -64,12 +79,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Roy Wang</author>
   </authors>
   <commentList>
-    <comment ref="S3" authorId="0" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -201,18 +216,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ &quot;¥&quot;* #,##0_ ;_ &quot;¥&quot;* \-#,##0_ ;_ &quot;¥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ &quot;¥&quot;* #,##0.00_ ;_ &quot;¥&quot;* \-#,##0.00_ ;_ &quot;¥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -226,7 +241,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -250,7 +265,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -282,37 +297,34 @@
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Comma" xfId="4"/>
-    <cellStyle name="Comma [0]" xfId="5"/>
-    <cellStyle name="Currency" xfId="2"/>
-    <cellStyle name="Currency [0]" xfId="3"/>
-    <cellStyle name="Hyperlink" xfId="6"/>
+    <cellStyle name="Comma" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma [0]" xfId="5" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Currency" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Currency [0]" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Hyperlink" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1"/>
+    <cellStyle name="Percent" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -397,7 +409,7 @@
               </a:solidFill>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -519,7 +531,7 @@
           </a:solidFill>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -566,7 +578,7 @@
               </a:solidFill>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -766,7 +778,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="27656436"/>
@@ -820,7 +832,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="43572788"/>
@@ -860,7 +872,7 @@
               <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -926,7 +938,7 @@
               </a:solidFill>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -982,7 +994,7 @@
                     </a:solidFill>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="zh-CN"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1178,7 +1190,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="41973208"/>
@@ -1232,7 +1244,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="56504966"/>
@@ -1269,7 +1281,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -1306,7 +1318,7 @@
               <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1372,7 +1384,7 @@
               </a:solidFill>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1635,7 +1647,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="59577537"/>
@@ -1689,7 +1701,7 @@
                 </a:solidFill>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="9987539"/>
@@ -1729,7 +1741,7 @@
               <a:cs typeface="Calibri"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1892,7 +1904,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4242,13 +4253,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{979F0D20-33BD-460B-AB47-9AE3C7708F6F}" type="pres">
       <dgm:prSet presAssocID="{8CBF365D-6451-4AB4-8C4E-5C70D33FD82F}" presName="node" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="2">
@@ -4257,13 +4261,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{5E0653FF-B751-4BEC-924E-422310E4C643}" type="pres">
       <dgm:prSet presAssocID="{02C8852D-A065-4324-BB00-0A1B28BE8DCA}" presName="sibTrans" presStyleCnt="0"/>
@@ -4276,21 +4273,14 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{A718B048-3E9B-4969-893D-AD8724E78C80}" srcId="{17B3D90C-A3DC-4821-A989-84B9B9918FDD}" destId="{8CBF365D-6451-4AB4-8C4E-5C70D33FD82F}" srcOrd="0" destOrd="0" parTransId="{48012BEF-5DF4-4294-BA72-D0B3CFDED756}" sibTransId="{02C8852D-A065-4324-BB00-0A1B28BE8DCA}"/>
+    <dgm:cxn modelId="{98038B84-B7DC-4245-B80A-262141BDEE08}" type="presOf" srcId="{17B3D90C-A3DC-4821-A989-84B9B9918FDD}" destId="{64039719-5727-48BA-8F5D-8469857C1056}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
+    <dgm:cxn modelId="{FC0E8B9B-3B09-4CF6-8DCE-27C7643F589C}" srcId="{17B3D90C-A3DC-4821-A989-84B9B9918FDD}" destId="{9B8C42A6-CBE5-4C4B-8519-906A6241A62F}" srcOrd="1" destOrd="0" parTransId="{2867A608-51C3-4E9F-80E0-03AC2ABAEB9E}" sibTransId="{16379AA1-32F2-474C-B05B-7409109A1784}"/>
     <dgm:cxn modelId="{9F30A19F-351D-4770-AAF0-04D3A2FD79FA}" type="presOf" srcId="{8CBF365D-6451-4AB4-8C4E-5C70D33FD82F}" destId="{979F0D20-33BD-460B-AB47-9AE3C7708F6F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{FC0E8B9B-3B09-4CF6-8DCE-27C7643F589C}" srcId="{17B3D90C-A3DC-4821-A989-84B9B9918FDD}" destId="{9B8C42A6-CBE5-4C4B-8519-906A6241A62F}" srcOrd="1" destOrd="0" parTransId="{2867A608-51C3-4E9F-80E0-03AC2ABAEB9E}" sibTransId="{16379AA1-32F2-474C-B05B-7409109A1784}"/>
-    <dgm:cxn modelId="{A718B048-3E9B-4969-893D-AD8724E78C80}" srcId="{17B3D90C-A3DC-4821-A989-84B9B9918FDD}" destId="{8CBF365D-6451-4AB4-8C4E-5C70D33FD82F}" srcOrd="0" destOrd="0" parTransId="{48012BEF-5DF4-4294-BA72-D0B3CFDED756}" sibTransId="{02C8852D-A065-4324-BB00-0A1B28BE8DCA}"/>
     <dgm:cxn modelId="{D1AA00F0-09A7-44CE-8C7A-428B8C52D5BA}" type="presOf" srcId="{9B8C42A6-CBE5-4C4B-8519-906A6241A62F}" destId="{5C25943E-09F9-4D35-8A3B-0E199ABC8277}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
-    <dgm:cxn modelId="{98038B84-B7DC-4245-B80A-262141BDEE08}" type="presOf" srcId="{17B3D90C-A3DC-4821-A989-84B9B9918FDD}" destId="{64039719-5727-48BA-8F5D-8469857C1056}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
     <dgm:cxn modelId="{4E2F3337-D882-4D3C-8203-7458F20FED98}" type="presParOf" srcId="{64039719-5727-48BA-8F5D-8469857C1056}" destId="{979F0D20-33BD-460B-AB47-9AE3C7708F6F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
     <dgm:cxn modelId="{AD1C3029-20CE-458C-96F4-77C162F93116}" type="presParOf" srcId="{64039719-5727-48BA-8F5D-8469857C1056}" destId="{5E0653FF-B751-4BEC-924E-422310E4C643}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
     <dgm:cxn modelId="{1B105D5F-40A3-469F-B040-731DBF5FE169}" type="presParOf" srcId="{64039719-5727-48BA-8F5D-8469857C1056}" destId="{5C25943E-09F9-4D35-8A3B-0E199ABC8277}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/default"/>
@@ -4527,13 +4517,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CC48429B-F451-4E09-B2C0-44AABE7123E6}" type="pres">
       <dgm:prSet presAssocID="{0A7DD416-267B-438D-B5DC-8845C764596E}" presName="composite" presStyleCnt="0"/>
@@ -4548,13 +4531,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{B930369B-D2A0-4F63-9F48-D9B1B51F9A4E}" type="pres">
       <dgm:prSet presAssocID="{0A7DD416-267B-438D-B5DC-8845C764596E}" presName="Childtext1" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="3">
@@ -4565,13 +4541,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{670F3B4A-51AC-4B63-BD33-0256D1007111}" type="pres">
       <dgm:prSet presAssocID="{0A7DD416-267B-438D-B5DC-8845C764596E}" presName="BalanceSpacing" presStyleCnt="0"/>
@@ -4584,13 +4553,6 @@
     <dgm:pt modelId="{53337A83-2C88-47CB-8EA7-8DEB9E392E35}" type="pres">
       <dgm:prSet presAssocID="{F0F745EA-804A-4F34-9449-9CFC1C48D517}" presName="Accent1Text" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="6"/>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{55EC2D5E-A238-40E8-B163-8A66FDE3EC39}" type="pres">
       <dgm:prSet presAssocID="{F0F745EA-804A-4F34-9449-9CFC1C48D517}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
@@ -4609,13 +4571,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{E69DED3E-1798-498A-B9A6-EC95C7494A6D}" type="pres">
       <dgm:prSet presAssocID="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" presName="Childtext1" presStyleLbl="revTx" presStyleIdx="1" presStyleCnt="3">
@@ -4626,13 +4581,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{A358E4FC-9AF1-416D-936F-71892D6F37AC}" type="pres">
       <dgm:prSet presAssocID="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" presName="BalanceSpacing" presStyleCnt="0"/>
@@ -4645,13 +4593,6 @@
     <dgm:pt modelId="{8FC7D08A-84F9-4114-9F68-EAA65B3092AA}" type="pres">
       <dgm:prSet presAssocID="{A727D898-45EF-4821-93A8-9861D04F77F4}" presName="Accent1Text" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="6"/>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0C252557-7C18-4EE9-9A50-52A6A026AE28}" type="pres">
       <dgm:prSet presAssocID="{A727D898-45EF-4821-93A8-9861D04F77F4}" presName="spaceBetweenRectangles" presStyleCnt="0"/>
@@ -4670,13 +4611,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F941179A-7E65-4142-A4DE-C77422569540}" type="pres">
       <dgm:prSet presAssocID="{6F590912-D5BE-43AA-9E77-BB33E52B30B8}" presName="Childtext1" presStyleLbl="revTx" presStyleIdx="2" presStyleCnt="3">
@@ -4687,13 +4621,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{DC0B7296-06F2-4DFA-A746-F394D5B41282}" type="pres">
       <dgm:prSet presAssocID="{6F590912-D5BE-43AA-9E77-BB33E52B30B8}" presName="BalanceSpacing" presStyleCnt="0"/>
@@ -4706,32 +4633,25 @@
     <dgm:pt modelId="{E548E58E-B118-4D34-9B17-B7C7F1C4A379}" type="pres">
       <dgm:prSet presAssocID="{A89C2BE1-6682-4A20-B065-FDEA4EED0285}" presName="Accent1Text" presStyleLbl="node1" presStyleIdx="5" presStyleCnt="6"/>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{D5EFC8F5-2DD7-4248-AB3F-D76B61A56501}" srcId="{937B6240-3360-4ADE-8EDE-D4773986ED6C}" destId="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" srcOrd="1" destOrd="0" parTransId="{B4BB156D-7651-41B2-B3AB-3EDA60B9D7DD}" sibTransId="{A727D898-45EF-4821-93A8-9861D04F77F4}"/>
-    <dgm:cxn modelId="{5E49E9EF-CB19-44B0-B640-A7F0203F464A}" type="presOf" srcId="{937B6240-3360-4ADE-8EDE-D4773986ED6C}" destId="{133E9812-3653-4405-A6C3-B32F475BF75B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{A1162218-BE2E-409C-9F16-59E43D5ECA82}" type="presOf" srcId="{A89C2BE1-6682-4A20-B065-FDEA4EED0285}" destId="{E548E58E-B118-4D34-9B17-B7C7F1C4A379}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{4B17A11B-4D33-4679-8ABC-0BF6AB33996E}" type="presOf" srcId="{0A7DD416-267B-438D-B5DC-8845C764596E}" destId="{8FACBB76-2B25-44A3-B84E-BD7272474957}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{BE92F930-D4EA-4770-8129-70B448EC51FA}" srcId="{0A7DD416-267B-438D-B5DC-8845C764596E}" destId="{59EDCD32-8D02-47F3-9DE7-8138633A80F2}" srcOrd="0" destOrd="0" parTransId="{9AB052ED-A57C-499C-860A-F908EC7B4FFE}" sibTransId="{BB411B71-DACD-492D-B2D5-1F944F310BB3}"/>
+    <dgm:cxn modelId="{46A3D33D-36B3-42F4-9DEE-1511EBDD3C3C}" type="presOf" srcId="{A727D898-45EF-4821-93A8-9861D04F77F4}" destId="{8FC7D08A-84F9-4114-9F68-EAA65B3092AA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{55F2AC42-F823-4614-9C12-CDFB9BD65F18}" srcId="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" destId="{E96D4E76-EDCA-47C9-8D08-F70299FE6A49}" srcOrd="0" destOrd="0" parTransId="{6EF3109F-D517-4CC0-900D-9A5AB72BCD8C}" sibTransId="{36DED21B-7471-41D1-A9FA-2DFBAC2CE978}"/>
+    <dgm:cxn modelId="{A669BD7A-0222-4A69-AF0B-37E46FA40732}" type="presOf" srcId="{F0F745EA-804A-4F34-9449-9CFC1C48D517}" destId="{53337A83-2C88-47CB-8EA7-8DEB9E392E35}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
     <dgm:cxn modelId="{16E2A980-D53B-4539-9D3F-3D73E1CF258C}" srcId="{6F590912-D5BE-43AA-9E77-BB33E52B30B8}" destId="{25A668DE-821B-4969-A830-AF29CB8A8E05}" srcOrd="0" destOrd="0" parTransId="{7B813D94-B076-4A13-91D6-70B03DCC2E74}" sibTransId="{2704066F-82FC-44A7-97D2-F0E2568B72F3}"/>
-    <dgm:cxn modelId="{A1162218-BE2E-409C-9F16-59E43D5ECA82}" type="presOf" srcId="{A89C2BE1-6682-4A20-B065-FDEA4EED0285}" destId="{E548E58E-B118-4D34-9B17-B7C7F1C4A379}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
-    <dgm:cxn modelId="{55F2AC42-F823-4614-9C12-CDFB9BD65F18}" srcId="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" destId="{E96D4E76-EDCA-47C9-8D08-F70299FE6A49}" srcOrd="0" destOrd="0" parTransId="{6EF3109F-D517-4CC0-900D-9A5AB72BCD8C}" sibTransId="{36DED21B-7471-41D1-A9FA-2DFBAC2CE978}"/>
-    <dgm:cxn modelId="{4B17A11B-4D33-4679-8ABC-0BF6AB33996E}" type="presOf" srcId="{0A7DD416-267B-438D-B5DC-8845C764596E}" destId="{8FACBB76-2B25-44A3-B84E-BD7272474957}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{5656B289-68EA-4DAD-B464-C6BB8878964A}" type="presOf" srcId="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" destId="{647BCE6B-49D9-4061-808E-497371A775C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{8D5FE096-92DD-4E49-8A52-42EC3A0A807A}" type="presOf" srcId="{59EDCD32-8D02-47F3-9DE7-8138633A80F2}" destId="{B930369B-D2A0-4F63-9F48-D9B1B51F9A4E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
     <dgm:cxn modelId="{31560DB2-9DB9-4CD5-B2F0-7309D4008BD5}" type="presOf" srcId="{25A668DE-821B-4969-A830-AF29CB8A8E05}" destId="{F941179A-7E65-4142-A4DE-C77422569540}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
     <dgm:cxn modelId="{B41D7FB3-8F43-4225-8F08-A4018DB0C417}" srcId="{937B6240-3360-4ADE-8EDE-D4773986ED6C}" destId="{0A7DD416-267B-438D-B5DC-8845C764596E}" srcOrd="0" destOrd="0" parTransId="{226FD3DE-244A-4E57-8450-83C128A2F848}" sibTransId="{F0F745EA-804A-4F34-9449-9CFC1C48D517}"/>
+    <dgm:cxn modelId="{0C04A9C6-7912-4BAB-8443-425C61541DAB}" type="presOf" srcId="{E96D4E76-EDCA-47C9-8D08-F70299FE6A49}" destId="{E69DED3E-1798-498A-B9A6-EC95C7494A6D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{3BFB39D0-A6C3-4F10-9243-E0DA710E7C5C}" type="presOf" srcId="{6F590912-D5BE-43AA-9E77-BB33E52B30B8}" destId="{B7F626B2-5CA0-4456-B060-5D90A1C6F809}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
     <dgm:cxn modelId="{2C3C80DB-D04F-4564-958A-E40A363F36A7}" srcId="{937B6240-3360-4ADE-8EDE-D4773986ED6C}" destId="{6F590912-D5BE-43AA-9E77-BB33E52B30B8}" srcOrd="2" destOrd="0" parTransId="{A19A4F95-A653-43EF-9C84-B58CED3F6111}" sibTransId="{A89C2BE1-6682-4A20-B065-FDEA4EED0285}"/>
-    <dgm:cxn modelId="{3BFB39D0-A6C3-4F10-9243-E0DA710E7C5C}" type="presOf" srcId="{6F590912-D5BE-43AA-9E77-BB33E52B30B8}" destId="{B7F626B2-5CA0-4456-B060-5D90A1C6F809}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
-    <dgm:cxn modelId="{8D5FE096-92DD-4E49-8A52-42EC3A0A807A}" type="presOf" srcId="{59EDCD32-8D02-47F3-9DE7-8138633A80F2}" destId="{B930369B-D2A0-4F63-9F48-D9B1B51F9A4E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
-    <dgm:cxn modelId="{46A3D33D-36B3-42F4-9DEE-1511EBDD3C3C}" type="presOf" srcId="{A727D898-45EF-4821-93A8-9861D04F77F4}" destId="{8FC7D08A-84F9-4114-9F68-EAA65B3092AA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
-    <dgm:cxn modelId="{BE92F930-D4EA-4770-8129-70B448EC51FA}" srcId="{0A7DD416-267B-438D-B5DC-8845C764596E}" destId="{59EDCD32-8D02-47F3-9DE7-8138633A80F2}" srcOrd="0" destOrd="0" parTransId="{9AB052ED-A57C-499C-860A-F908EC7B4FFE}" sibTransId="{BB411B71-DACD-492D-B2D5-1F944F310BB3}"/>
-    <dgm:cxn modelId="{0C04A9C6-7912-4BAB-8443-425C61541DAB}" type="presOf" srcId="{E96D4E76-EDCA-47C9-8D08-F70299FE6A49}" destId="{E69DED3E-1798-498A-B9A6-EC95C7494A6D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
-    <dgm:cxn modelId="{5656B289-68EA-4DAD-B464-C6BB8878964A}" type="presOf" srcId="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" destId="{647BCE6B-49D9-4061-808E-497371A775C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
-    <dgm:cxn modelId="{A669BD7A-0222-4A69-AF0B-37E46FA40732}" type="presOf" srcId="{F0F745EA-804A-4F34-9449-9CFC1C48D517}" destId="{53337A83-2C88-47CB-8EA7-8DEB9E392E35}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{5E49E9EF-CB19-44B0-B640-A7F0203F464A}" type="presOf" srcId="{937B6240-3360-4ADE-8EDE-D4773986ED6C}" destId="{133E9812-3653-4405-A6C3-B32F475BF75B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
+    <dgm:cxn modelId="{D5EFC8F5-2DD7-4248-AB3F-D76B61A56501}" srcId="{937B6240-3360-4ADE-8EDE-D4773986ED6C}" destId="{2061FF1F-889B-496D-80F8-C5CB3E9B64B5}" srcOrd="1" destOrd="0" parTransId="{B4BB156D-7651-41B2-B3AB-3EDA60B9D7DD}" sibTransId="{A727D898-45EF-4821-93A8-9861D04F77F4}"/>
     <dgm:cxn modelId="{83A16E8A-ED51-4BDD-B3B7-06A6E7CB8504}" type="presParOf" srcId="{133E9812-3653-4405-A6C3-B32F475BF75B}" destId="{CC48429B-F451-4E09-B2C0-44AABE7123E6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
     <dgm:cxn modelId="{78B690BC-418E-4E6E-8F44-3B5EDFF7A6D6}" type="presParOf" srcId="{CC48429B-F451-4E09-B2C0-44AABE7123E6}" destId="{8FACBB76-2B25-44A3-B84E-BD7272474957}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
     <dgm:cxn modelId="{7FE52DBE-B795-4D84-9CE3-2781638C3785}" type="presParOf" srcId="{CC48429B-F451-4E09-B2C0-44AABE7123E6}" destId="{B930369B-D2A0-4F63-9F48-D9B1B51F9A4E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2008/layout/AlternatingHexagons"/>
@@ -4885,13 +4805,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{B0320D0B-10EB-45B8-94E1-3C7F7AE4E307}" type="pres">
       <dgm:prSet presAssocID="{59530A0A-646A-446E-BE01-D9043C2613FE}" presName="parentLin" presStyleCnt="0"/>
@@ -4900,13 +4813,6 @@
     <dgm:pt modelId="{CD9B478D-C025-4DFC-ACD5-5A7DE2A5D8F4}" type="pres">
       <dgm:prSet presAssocID="{59530A0A-646A-446E-BE01-D9043C2613FE}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="3"/>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C24A3DE1-56D3-4C6F-B5DE-2BBD124CF73F}" type="pres">
       <dgm:prSet presAssocID="{59530A0A-646A-446E-BE01-D9043C2613FE}" presName="parentText" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="3">
@@ -4916,13 +4822,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{4A173A80-5438-494E-8360-509879831BC5}" type="pres">
       <dgm:prSet presAssocID="{59530A0A-646A-446E-BE01-D9043C2613FE}" presName="negativeSpace" presStyleCnt="0"/>
@@ -4947,13 +4846,6 @@
     <dgm:pt modelId="{9BA3B05C-9FD4-4BB6-8232-1E7950B115FF}" type="pres">
       <dgm:prSet presAssocID="{44D90809-E3DA-4031-88F2-962F46943481}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="3"/>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8CCB5DC3-BBBB-44CF-9B65-E99F1EA27F21}" type="pres">
       <dgm:prSet presAssocID="{44D90809-E3DA-4031-88F2-962F46943481}" presName="parentText" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="3">
@@ -4963,13 +4855,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{D5399B35-E93B-4C0C-A086-EB27500C9510}" type="pres">
       <dgm:prSet presAssocID="{44D90809-E3DA-4031-88F2-962F46943481}" presName="negativeSpace" presStyleCnt="0"/>
@@ -4994,13 +4879,6 @@
     <dgm:pt modelId="{6700AB4D-9505-4E86-B69E-86F6DC144205}" type="pres">
       <dgm:prSet presAssocID="{086564D8-D4C3-47FA-B165-2B8319F37810}" presName="parentLeftMargin" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="3"/>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{B39B8090-AA43-4B2C-BD14-6F0B5C09353B}" type="pres">
       <dgm:prSet presAssocID="{086564D8-D4C3-47FA-B165-2B8319F37810}" presName="parentText" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="3">
@@ -5010,13 +4888,6 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{4E88657B-C263-4CB5-8FDF-0720A7ECD72E}" type="pres">
       <dgm:prSet presAssocID="{086564D8-D4C3-47FA-B165-2B8319F37810}" presName="negativeSpace" presStyleCnt="0"/>
@@ -5032,16 +4903,16 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{9EBCFA3D-6A5A-4829-8256-AD2CD12F16AA}" srcId="{CC6C05E7-7A7F-4427-9EC4-052FACAF2511}" destId="{44D90809-E3DA-4031-88F2-962F46943481}" srcOrd="1" destOrd="0" parTransId="{147009AE-5945-47C3-8DBB-10E173FA6903}" sibTransId="{A6857444-0CC7-4F50-87F9-EB1FA752219D}"/>
+    <dgm:cxn modelId="{13D8AF63-9AE5-424B-868D-11D40486A651}" type="presOf" srcId="{086564D8-D4C3-47FA-B165-2B8319F37810}" destId="{6700AB4D-9505-4E86-B69E-86F6DC144205}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{59707252-B4CE-4E43-9CA6-642CD848C198}" type="presOf" srcId="{59530A0A-646A-446E-BE01-D9043C2613FE}" destId="{CD9B478D-C025-4DFC-ACD5-5A7DE2A5D8F4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
     <dgm:cxn modelId="{A5606D7A-3E4A-4CB7-91BC-8C2429AD8FD3}" type="presOf" srcId="{086564D8-D4C3-47FA-B165-2B8319F37810}" destId="{B39B8090-AA43-4B2C-BD14-6F0B5C09353B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{9182C58A-FD69-4B88-A89E-43EF76BB9340}" type="presOf" srcId="{CC6C05E7-7A7F-4427-9EC4-052FACAF2511}" destId="{3B4048B0-79DF-43DB-85C3-FED765AB95BE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{9DBD81B1-CB37-4BE2-A9C8-07BD666B3983}" type="presOf" srcId="{44D90809-E3DA-4031-88F2-962F46943481}" destId="{8CCB5DC3-BBBB-44CF-9B65-E99F1EA27F21}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
+    <dgm:cxn modelId="{2EF362CD-689E-46ED-8923-2E61D9F293EC}" type="presOf" srcId="{44D90809-E3DA-4031-88F2-962F46943481}" destId="{9BA3B05C-9FD4-4BB6-8232-1E7950B115FF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
     <dgm:cxn modelId="{9410C5E3-6AB1-4A05-A5CF-D99B1CD47D3A}" srcId="{CC6C05E7-7A7F-4427-9EC4-052FACAF2511}" destId="{086564D8-D4C3-47FA-B165-2B8319F37810}" srcOrd="2" destOrd="0" parTransId="{D7D86EA6-BE8F-403A-928D-38EEEEE8DF39}" sibTransId="{7D7C00FE-8B1D-476C-8460-00389DE4AF08}"/>
+    <dgm:cxn modelId="{C97B1CEE-C3A4-4E43-BB62-BB11AFB4FCBB}" type="presOf" srcId="{59530A0A-646A-446E-BE01-D9043C2613FE}" destId="{C24A3DE1-56D3-4C6F-B5DE-2BBD124CF73F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
     <dgm:cxn modelId="{9D0E38F4-79E8-4D11-88B1-2233228ACBE5}" srcId="{CC6C05E7-7A7F-4427-9EC4-052FACAF2511}" destId="{59530A0A-646A-446E-BE01-D9043C2613FE}" srcOrd="0" destOrd="0" parTransId="{4511DE0A-D837-4FD9-8CD0-B966DAD95312}" sibTransId="{3A30166D-43A6-4B06-877F-294747EF7208}"/>
-    <dgm:cxn modelId="{9182C58A-FD69-4B88-A89E-43EF76BB9340}" type="presOf" srcId="{CC6C05E7-7A7F-4427-9EC4-052FACAF2511}" destId="{3B4048B0-79DF-43DB-85C3-FED765AB95BE}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
-    <dgm:cxn modelId="{2EF362CD-689E-46ED-8923-2E61D9F293EC}" type="presOf" srcId="{44D90809-E3DA-4031-88F2-962F46943481}" destId="{9BA3B05C-9FD4-4BB6-8232-1E7950B115FF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
-    <dgm:cxn modelId="{C97B1CEE-C3A4-4E43-BB62-BB11AFB4FCBB}" type="presOf" srcId="{59530A0A-646A-446E-BE01-D9043C2613FE}" destId="{C24A3DE1-56D3-4C6F-B5DE-2BBD124CF73F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
-    <dgm:cxn modelId="{59707252-B4CE-4E43-9CA6-642CD848C198}" type="presOf" srcId="{59530A0A-646A-446E-BE01-D9043C2613FE}" destId="{CD9B478D-C025-4DFC-ACD5-5A7DE2A5D8F4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
-    <dgm:cxn modelId="{9DBD81B1-CB37-4BE2-A9C8-07BD666B3983}" type="presOf" srcId="{44D90809-E3DA-4031-88F2-962F46943481}" destId="{8CCB5DC3-BBBB-44CF-9B65-E99F1EA27F21}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
-    <dgm:cxn modelId="{13D8AF63-9AE5-424B-868D-11D40486A651}" type="presOf" srcId="{086564D8-D4C3-47FA-B165-2B8319F37810}" destId="{6700AB4D-9505-4E86-B69E-86F6DC144205}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
-    <dgm:cxn modelId="{9EBCFA3D-6A5A-4829-8256-AD2CD12F16AA}" srcId="{CC6C05E7-7A7F-4427-9EC4-052FACAF2511}" destId="{44D90809-E3DA-4031-88F2-962F46943481}" srcOrd="1" destOrd="0" parTransId="{147009AE-5945-47C3-8DBB-10E173FA6903}" sibTransId="{A6857444-0CC7-4F50-87F9-EB1FA752219D}"/>
     <dgm:cxn modelId="{7A80F35A-1B31-4143-BE27-F8DE30E45972}" type="presParOf" srcId="{3B4048B0-79DF-43DB-85C3-FED765AB95BE}" destId="{B0320D0B-10EB-45B8-94E1-3C7F7AE4E307}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
     <dgm:cxn modelId="{E8C728D1-62C2-4F9C-AAEA-9B7DEC31FED3}" type="presParOf" srcId="{B0320D0B-10EB-45B8-94E1-3C7F7AE4E307}" destId="{CD9B478D-C025-4DFC-ACD5-5A7DE2A5D8F4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
     <dgm:cxn modelId="{E9A371B7-41F9-46E4-9FDD-EA21780D70CD}" type="presParOf" srcId="{B0320D0B-10EB-45B8-94E1-3C7F7AE4E307}" destId="{C24A3DE1-56D3-4C6F-B5DE-2BBD124CF73F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/list1"/>
@@ -5132,7 +5003,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="2044700">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="2044700">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5142,6 +5013,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="4600" kern="1200"/>
@@ -5208,7 +5080,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="2044700">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="2044700">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5218,6 +5090,7 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="4600" kern="1200"/>
@@ -5249,8 +5122,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2374498" y="60888"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="2004230" y="67577"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5294,12 +5167,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="57150" tIns="57150" rIns="57150" bIns="57150" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="666750">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5309,13 +5182,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2558444" y="144190"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="2207964" y="159842"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B930369B-D2A0-4F63-9F48-D9B1B51F9A4E}">
@@ -5325,8 +5199,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3256190" y="184695"/>
-          <a:ext cx="1023473" cy="550254"/>
+          <a:off x="2980774" y="204704"/>
+          <a:ext cx="1133579" cy="609451"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5350,12 +5224,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="95250" tIns="95250" rIns="95250" bIns="95250" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="106680" tIns="106680" rIns="106680" bIns="106680" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="l" defTabSz="1111250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1244600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5365,13 +5239,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="2500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3256190" y="184695"/>
-        <a:ext cx="1023473" cy="550254"/>
+        <a:off x="2980774" y="204704"/>
+        <a:ext cx="1133579" cy="609451"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{53337A83-2C88-47CB-8EA7-8DEB9E392E35}">
@@ -5381,8 +5256,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1512799" y="60888"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="1049829" y="67577"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5431,7 +5306,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1600200">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5441,13 +5316,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-US" sz="3600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="1696745" y="144190"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="1253563" y="159842"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{647BCE6B-49D9-4061-808E-497371A775C8}">
@@ -5457,8 +5333,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1941998" y="839315"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="1525201" y="929747"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5502,12 +5378,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="57150" tIns="57150" rIns="57150" bIns="57150" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="666750">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5517,13 +5393,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2125944" y="922617"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="1728935" y="1022012"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E69DED3E-1798-498A-B9A6-EC95C7494A6D}">
@@ -5533,8 +5410,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="978135" y="963122"/>
-          <a:ext cx="990458" cy="550254"/>
+          <a:off x="457646" y="1066874"/>
+          <a:ext cx="1097012" cy="609451"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5558,12 +5435,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="95250" tIns="95250" rIns="95250" bIns="95250" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="106680" tIns="106680" rIns="106680" bIns="106680" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="r" defTabSz="1111250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="r" defTabSz="1244600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5573,13 +5450,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="2500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="978135" y="963122"/>
-        <a:ext cx="990458" cy="550254"/>
+        <a:off x="457646" y="1066874"/>
+        <a:ext cx="1097012" cy="609451"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8FC7D08A-84F9-4114-9F68-EAA65B3092AA}">
@@ -5589,8 +5467,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2803697" y="839315"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="2479602" y="929747"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5639,7 +5517,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1600200">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5649,13 +5527,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-US" sz="3600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2987643" y="922617"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="2683336" y="1022012"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{B7F626B2-5CA0-4456-B060-5D90A1C6F809}">
@@ -5665,8 +5544,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2374498" y="1617742"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="2004230" y="1791918"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5710,12 +5589,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="57150" tIns="57150" rIns="57150" bIns="57150" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="60960" tIns="60960" rIns="60960" bIns="60960" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="666750">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="711200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5725,13 +5604,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="1600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="2558444" y="1701044"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="2207964" y="1884183"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F941179A-7E65-4142-A4DE-C77422569540}">
@@ -5741,8 +5621,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3256190" y="1741549"/>
-          <a:ext cx="1023473" cy="550254"/>
+          <a:off x="2980774" y="1929044"/>
+          <a:ext cx="1133579" cy="609451"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5766,12 +5646,12 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="95250" tIns="95250" rIns="95250" bIns="95250" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="106680" tIns="106680" rIns="106680" bIns="106680" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="l" defTabSz="1111250">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="1244600">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5781,13 +5661,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="2500" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2800" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3256190" y="1741549"/>
-        <a:ext cx="1023473" cy="550254"/>
+        <a:off x="2980774" y="1929044"/>
+        <a:ext cx="1133579" cy="609451"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{E548E58E-B118-4D34-9B17-B7C7F1C4A379}">
@@ -5797,8 +5678,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="1512799" y="1617742"/>
-          <a:ext cx="917091" cy="797869"/>
+          <a:off x="1049829" y="1791918"/>
+          <a:ext cx="1015751" cy="883704"/>
         </a:xfrm>
         <a:prstGeom prst="hexagon">
           <a:avLst>
@@ -5847,7 +5728,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1600200">
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="1600200">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5857,13 +5738,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
           <a:endParaRPr lang="en-US" sz="3600" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-5400000">
-        <a:off x="1696745" y="1701044"/>
-        <a:ext cx="549199" cy="631265"/>
+        <a:off x="1253563" y="1884183"/>
+        <a:ext cx="608282" cy="699175"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -5885,8 +5767,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="327810"/>
-          <a:ext cx="5257800" cy="453600"/>
+          <a:off x="0" y="359999"/>
+          <a:ext cx="4572000" cy="504000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5933,8 +5815,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="262890" y="62130"/>
-          <a:ext cx="3680460" cy="531360"/>
+          <a:off x="228600" y="64799"/>
+          <a:ext cx="3200400" cy="590400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -5975,12 +5857,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="139113" tIns="0" rIns="139113" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="l" defTabSz="800100">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -5990,13 +5872,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="288829" y="88069"/>
-        <a:ext cx="3628582" cy="479482"/>
+        <a:off x="257421" y="93620"/>
+        <a:ext cx="3142758" cy="532758"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9A40B308-CE02-4B71-BA70-C0D200CBD383}">
@@ -6006,8 +5889,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="1144290"/>
-          <a:ext cx="5257800" cy="453600"/>
+          <a:off x="0" y="1267200"/>
+          <a:ext cx="4572000" cy="504000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6054,8 +5937,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="262890" y="878610"/>
-          <a:ext cx="3680460" cy="531360"/>
+          <a:off x="228600" y="972000"/>
+          <a:ext cx="3200400" cy="590400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6096,12 +5979,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="139113" tIns="0" rIns="139113" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="l" defTabSz="800100">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6111,13 +5994,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="288829" y="904549"/>
-        <a:ext cx="3628582" cy="479482"/>
+        <a:off x="257421" y="1000821"/>
+        <a:ext cx="3142758" cy="532758"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{BE4CD07D-369F-49DD-8139-FD09651870C8}">
@@ -6127,8 +6011,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="0" y="1960770"/>
-          <a:ext cx="5257800" cy="453600"/>
+          <a:off x="0" y="2174400"/>
+          <a:ext cx="4572000" cy="504000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6175,8 +6059,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="262890" y="1695090"/>
-          <a:ext cx="3680460" cy="531360"/>
+          <a:off x="228600" y="1879200"/>
+          <a:ext cx="3200400" cy="590400"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -6217,12 +6101,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="139113" tIns="0" rIns="139113" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="120968" tIns="0" rIns="120968" bIns="0" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="l" defTabSz="800100">
+          <a:pPr marL="0" lvl="0" indent="0" algn="l" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -6232,13 +6116,14 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
+            <a:buNone/>
           </a:pPr>
-          <a:endParaRPr lang="en-US" sz="1800" kern="1200"/>
+          <a:endParaRPr lang="en-US" sz="2000" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="288829" y="1721029"/>
-        <a:ext cx="3628582" cy="479482"/>
+        <a:off x="257421" y="1908021"/>
+        <a:ext cx="3142758" cy="532758"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -10091,7 +9976,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10121,7 +10012,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Oval 4"/>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10182,7 +10079,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagram 5"/>
+        <xdr:cNvPr id="6" name="Diagram 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10212,7 +10115,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10242,7 +10151,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10272,7 +10187,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -10314,6 +10235,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4098"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -10329,11 +10253,10 @@
             <a:solidFill>
               <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
             </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -10367,6 +10290,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4100"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -10382,11 +10308,10 @@
             <a:solidFill>
               <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
             </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -10420,6 +10345,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4101"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -10435,11 +10363,10 @@
             <a:solidFill>
               <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
             </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -10466,7 +10393,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10530,7 +10463,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Straight Connector 3"/>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10582,7 +10521,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10643,7 +10588,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Smiley Face 5"/>
+        <xdr:cNvPr id="6" name="Smiley Face 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10704,7 +10655,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Curved Right Arrow 6"/>
+        <xdr:cNvPr id="7" name="Curved Right Arrow 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10769,7 +10726,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Plus 7"/>
+        <xdr:cNvPr id="8" name="Plus 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10830,7 +10793,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="Flowchart: Process 8"/>
+        <xdr:cNvPr id="9" name="Flowchart: Process 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10891,7 +10860,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Explosion 1 9"/>
+        <xdr:cNvPr id="10" name="Explosion 1 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10952,7 +10927,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Rectangular Callout 10"/>
+        <xdr:cNvPr id="11" name="Rectangular Callout 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11013,7 +10994,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11060,7 +11047,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -11102,7 +11095,13 @@
     <xdr:ext cx="4305300" cy="933450"/>
     <xdr:sp macro="" textlink="" fLocksText="0">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="Rectangle 16"/>
+        <xdr:cNvPr id="17" name="Rectangle 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11178,6 +11177,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4102"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006100000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -11193,11 +11195,10 @@
             <a:solidFill>
               <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
             </a:solidFill>
-            <a:ln w="9525" cmpd="sng">
+            <a:ln w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
               <a:miter lim="800000"/>
               <a:headEnd/>
               <a:tailEnd/>
@@ -11224,7 +11225,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Diagram 2"/>
+        <xdr:cNvPr id="3" name="Diagram 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -11254,7 +11261,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="12" name="Diagram 11"/>
+        <xdr:cNvPr id="12" name="Diagram 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -11284,7 +11297,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvPr id="13" name="Chart 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -11302,30 +11321,85 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{941E4FC8-CC1D-4230-B574-74FEBC8A88D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="409575" y="514350"/>
+          <a:ext cx="3171825" cy="1924050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C3:I23" totalsRowShown="0">
-  <autoFilter ref="C3:I23"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="C3:I23" totalsRowShown="0">
+  <autoFilter ref="C3:I23" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Column1"/>
-    <tableColumn id="2" name="Column2"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
-    <tableColumn id="5" name="Column5"/>
-    <tableColumn id="6" name="Column6"/>
-    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Column6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Column7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="M6:P10" totalsRowShown="0">
-  <autoFilter ref="M6:P10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="M6:P10" totalsRowShown="0">
+  <autoFilter ref="M6:P10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Column1" dataDxfId="1"/>
-    <tableColumn id="2" name="Column2" dataDxfId="0"/>
-    <tableColumn id="3" name="Column3"/>
-    <tableColumn id="4" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11407,6 +11481,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -11442,6 +11533,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -11617,23 +11725,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+    <row r="2" spans="2:20">
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:20">
       <c r="B3">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:20">
       <c r="I5">
         <v>1</v>
       </c>
@@ -11644,7 +11752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:20">
       <c r="I6">
         <v>10</v>
       </c>
@@ -11655,71 +11763,71 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
+    <row r="7" spans="2:20">
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
     </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:20">
       <c r="D11">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="1"/>
+    <row r="13" spans="2:20">
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="1"/>
+    <row r="14" spans="2:20">
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="1"/>
+    <row r="15" spans="2:20">
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
     </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.15">
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="1"/>
+    <row r="16" spans="2:20">
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
     </row>
-    <row r="17" spans="18:20" x14ac:dyDescent="0.15">
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="1"/>
+    <row r="17" spans="18:20">
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
     </row>
-    <row r="18" spans="18:20" x14ac:dyDescent="0.15">
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
+    <row r="18" spans="18:20">
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
     </row>
-    <row r="19" spans="18:20" x14ac:dyDescent="0.15">
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
+    <row r="19" spans="18:20">
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="5:5">
       <c r="E35" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="5:5">
       <c r="E36" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="5:5">
       <c r="E37" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="5:5">
       <c r="E38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="5:5">
       <c r="E39" s="2" t="s">
         <v>6</v>
       </c>
@@ -11778,20 +11886,20 @@
     <cfRule type="top10" dxfId="2" priority="1" percent="1" rank="10"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>I5</formula1>
       <formula2>K6</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="error alert" error="error message" promptTitle="test input" sqref="D11">
+    <dataValidation type="whole" operator="lessThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="error alert" error="error message" promptTitle="test input" sqref="D11" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>K6</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E35" r:id="rId1"/>
-    <hyperlink ref="E36" r:id="rId2"/>
-    <hyperlink ref="E37" r:id="rId3"/>
-    <hyperlink ref="E39" r:id="rId4"/>
-    <hyperlink ref="E38" r:id="rId5"/>
+    <hyperlink ref="E35" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E36" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E37" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E39" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E38" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -11825,25 +11933,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B5:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="6" max="7" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="C5" s="4"/>
+    <row r="5" spans="2:8">
+      <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+    <row r="6" spans="2:8">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
     </row>
-    <row r="8" spans="2:8" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8">
       <c r="G8" t="s">
         <v>3</v>
       </c>
@@ -11851,23 +11959,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="F10" s="5">
+    <row r="10" spans="2:8">
+      <c r="F10" s="4">
         <f ca="1">NOW()</f>
-        <v>42839.594554976851</v>
+        <v>44939.719515277779</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+    <row r="12" spans="2:8">
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="13" spans="2:8">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+    <row r="14" spans="2:8">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11881,14 +11989,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="E15:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="15" spans="5:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="5:6">
       <c r="E15" t="s">
         <v>7</v>
       </c>
@@ -11896,7 +12004,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="5:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="5:6">
       <c r="E16" t="s">
         <v>9</v>
       </c>
@@ -11904,7 +12012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.15">
+    <row r="17" spans="5:6">
       <c r="E17" t="s">
         <v>12</v>
       </c>
@@ -11912,7 +12020,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="5:6">
       <c r="E18" t="s">
         <v>8</v>
       </c>
@@ -11920,7 +12028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="5:6">
       <c r="E19" t="s">
         <v>11</v>
       </c>
@@ -11928,7 +12036,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="5:6">
       <c r="E20" t="s">
         <v>15</v>
       </c>
@@ -11936,7 +12044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="5:6">
       <c r="E21" t="s">
         <v>12</v>
       </c>
@@ -11953,14 +12061,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="C7:D11"/>
   <sheetViews>
     <sheetView topLeftCell="B43" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="3:4">
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -11968,7 +12076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="3:4">
       <c r="C8">
         <v>1</v>
       </c>
@@ -11976,7 +12084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="3:4">
       <c r="C9">
         <v>2</v>
       </c>
@@ -11984,7 +12092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="3:4">
       <c r="C10">
         <v>3</v>
       </c>
@@ -11992,7 +12100,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="3:4">
       <c r="C11">
         <v>4</v>
       </c>
@@ -12010,18 +12118,18 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="B3:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:5">
       <c r="B3" t="s">
         <v>25</v>
       </c>
@@ -12035,11 +12143,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="6">
+    <row r="4" spans="2:5" hidden="1">
+      <c r="B4" s="5">
         <v>41244</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>0.4236111111111111</v>
       </c>
       <c r="D4" t="s">
@@ -12049,11 +12157,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="6">
+    <row r="5" spans="2:5" hidden="1">
+      <c r="B5" s="5">
         <v>41245</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>0.46527777777777801</v>
       </c>
       <c r="D5" t="s">
@@ -12063,11 +12171,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="6">
+    <row r="6" spans="2:5" hidden="1">
+      <c r="B6" s="5">
         <v>41246</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>0.50694444444444398</v>
       </c>
       <c r="D6" t="s">
@@ -12077,11 +12185,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="6">
+    <row r="7" spans="2:5" hidden="1">
+      <c r="B7" s="5">
         <v>41247</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.54861111111111105</v>
       </c>
       <c r="D7" t="s">
@@ -12091,11 +12199,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="6">
+    <row r="8" spans="2:5" hidden="1">
+      <c r="B8" s="5">
         <v>41248</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6">
         <v>0.59027777777777801</v>
       </c>
       <c r="D8" t="s">
@@ -12105,11 +12213,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B9" s="6">
+    <row r="9" spans="2:5">
+      <c r="B9" s="5">
         <v>41249</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6">
         <v>0.63194444444444398</v>
       </c>
       <c r="D9" t="s">
@@ -12119,11 +12227,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B10" s="6">
+    <row r="10" spans="2:5">
+      <c r="B10" s="5">
         <v>41250</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>0.67361111111111105</v>
       </c>
       <c r="D10" t="s">
@@ -12133,11 +12241,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B11" s="6">
+    <row r="11" spans="2:5">
+      <c r="B11" s="5">
         <v>41251</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>0.71527777777777801</v>
       </c>
       <c r="D11" t="s">
@@ -12147,11 +12255,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B12" s="6">
+    <row r="12" spans="2:5">
+      <c r="B12" s="5">
         <v>41252</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6">
         <v>0.75694444444444398</v>
       </c>
       <c r="D12" t="s">
@@ -12161,11 +12269,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B13" s="6">
+    <row r="13" spans="2:5">
+      <c r="B13" s="5">
         <v>41253</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6">
         <v>0.79861111111111105</v>
       </c>
       <c r="D13" t="s">
@@ -12175,11 +12283,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B14" s="6">
+    <row r="14" spans="2:5">
+      <c r="B14" s="5">
         <v>41254</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6">
         <v>0.84027777777777801</v>
       </c>
       <c r="D14" t="s">
@@ -12189,11 +12297,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B15" s="6">
+    <row r="15" spans="2:5">
+      <c r="B15" s="5">
         <v>41255</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="6">
         <v>0.88194444444444398</v>
       </c>
       <c r="D15" t="s">
@@ -12203,11 +12311,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B16" s="6">
+    <row r="16" spans="2:5">
+      <c r="B16" s="5">
         <v>41256</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6">
         <v>0.92361111111111105</v>
       </c>
       <c r="D16" t="s">
@@ -12217,11 +12325,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B17" s="6">
+    <row r="17" spans="2:5">
+      <c r="B17" s="5">
         <v>41257</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>0.96527777777777801</v>
       </c>
       <c r="D17" t="s">
@@ -12231,11 +12339,11 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.15">
-      <c r="B18" s="6">
+    <row r="18" spans="2:5">
+      <c r="B18" s="5">
         <v>41258</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>1.00694444444444</v>
       </c>
       <c r="D18" t="s">
@@ -12246,7 +12354,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B3:E18">
+  <autoFilter ref="B3:E18" xr:uid="{00000000-0009-0000-0000-000004000000}">
     <filterColumn colId="3">
       <top10 val="10" filterVal="6"/>
     </filterColumn>
@@ -12266,15 +12374,15 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="S3:AC14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="19:29" x14ac:dyDescent="0.15"/>
-    <row r="13" spans="19:29" x14ac:dyDescent="0.15">
+    <row r="3" spans="19:29"/>
+    <row r="13" spans="19:29">
       <c r="AA13">
         <v>1</v>
       </c>
@@ -12285,7 +12393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="19:29" x14ac:dyDescent="0.15">
+    <row r="14" spans="19:29">
       <c r="AA14">
         <v>4</v>
       </c>
@@ -12408,18 +12516,31 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C802F16A-C50B-482A-860E-AEA43686CD41}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="C3:P23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="9" width="10.875" customWidth="1"/>
-    <col min="13" max="16" width="10.875" customWidth="1"/>
+    <col min="3" max="9" width="10.85546875" customWidth="1"/>
+    <col min="13" max="16" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="3:16">
       <c r="C3" t="s">
         <v>29</v>
       </c>
@@ -12442,7 +12563,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="3:16">
       <c r="C4">
         <v>1</v>
       </c>
@@ -12465,7 +12586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="3:16">
       <c r="C5">
         <v>2</v>
       </c>
@@ -12488,7 +12609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="3:16">
       <c r="C6">
         <v>3</v>
       </c>
@@ -12510,10 +12631,10 @@
       <c r="I6">
         <v>3</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O6" t="s">
@@ -12523,7 +12644,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="3:16">
       <c r="C7">
         <v>4</v>
       </c>
@@ -12545,10 +12666,10 @@
       <c r="I7">
         <v>4</v>
       </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="3:16">
       <c r="C8">
         <v>5</v>
       </c>
@@ -12570,10 +12691,10 @@
       <c r="I8">
         <v>5</v>
       </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="3:16">
       <c r="C9">
         <v>6</v>
       </c>
@@ -12595,10 +12716,10 @@
       <c r="I9">
         <v>6</v>
       </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="3:16">
       <c r="C10">
         <v>7</v>
       </c>
@@ -12620,10 +12741,10 @@
       <c r="I10">
         <v>7</v>
       </c>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="11" spans="3:16">
       <c r="C11">
         <v>8</v>
       </c>
@@ -12646,7 +12767,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="12" spans="3:16">
       <c r="C12">
         <v>9</v>
       </c>
@@ -12669,7 +12790,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="13" spans="3:16">
       <c r="C13">
         <v>10</v>
       </c>
@@ -12692,7 +12813,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="14" spans="3:16">
       <c r="C14">
         <v>11</v>
       </c>
@@ -12715,7 +12836,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="15" spans="3:16">
       <c r="C15">
         <v>12</v>
       </c>
@@ -12738,7 +12859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.15">
+    <row r="16" spans="3:16">
       <c r="C16">
         <v>13</v>
       </c>
@@ -12761,7 +12882,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:9">
       <c r="C17">
         <v>14</v>
       </c>
@@ -12784,7 +12905,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:9">
       <c r="C18">
         <v>15</v>
       </c>
@@ -12807,7 +12928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:9">
       <c r="C19">
         <v>16</v>
       </c>
@@ -12830,7 +12951,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:9">
       <c r="C20">
         <v>17</v>
       </c>
@@ -12853,7 +12974,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:9">
       <c r="C21">
         <v>18</v>
       </c>
@@ -12876,7 +12997,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="22" spans="3:9">
       <c r="C22">
         <v>19</v>
       </c>
@@ -12899,7 +13020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.15">
+    <row r="23" spans="3:9">
       <c r="C23">
         <v>20</v>
       </c>
@@ -12934,13 +13055,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>